<commit_message>
Avaliação de code smells otimizado
Co-Authored-By: dianamml17 <73841693+dianamml17@users.noreply.github.com>
Co-Authored-By: dcandeias20 <78976610+dcandeias20@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Code_Smells.xlsx
+++ b/Code_Smells.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iscteiul365-my.sharepoint.com/personal/dfbcs_iscte-iul_pt/Documents/eclipse-workspace/ES-2Sem-2021-Grupo-5/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{B5760989-AF68-4A21-B397-4D29D5B702E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{CECACAAB-5218-465B-922D-3D33F97D3ACD}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="2610" yWindow="2640" windowWidth="21600" windowHeight="11385" xr2:uid="{00B73718-A218-4BB5-A155-7549172451AD}"/>
+    <workbookView xWindow="2610" yWindow="2640" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Code Smells" sheetId="8" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -918,8 +912,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -929,6 +923,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -956,12 +958,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -994,7 +998,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37BC1AD5-7A45-4A8A-949C-97B741A8E176}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37BC1AD5-7A45-4A8A-949C-97B741A8E176}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1328,19 +1332,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43A618D-78EA-49A9-8234-7C33B19D7EFA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:K248"/>
+  <dimension ref="A1:P248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,9 +1357,10 @@
     <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>291</v>
       </c>
@@ -1390,7 +1395,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1425,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1460,7 +1465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1495,7 +1500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1530,7 +1535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1565,7 +1570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1599,8 +1604,9 @@
       <c r="K7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="P7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1635,7 +1641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1670,7 +1676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1705,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1740,7 +1746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1775,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1810,7 +1816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1845,7 +1851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1880,7 +1886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1915,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1950,7 +1956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1985,7 +1991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2020,7 +2026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2055,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2090,7 +2096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2125,7 +2131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2160,7 +2166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2195,7 +2201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2230,7 +2236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2265,7 +2271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2300,7 +2306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2334,8 +2340,9 @@
       <c r="K28" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="O28" s="4"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2370,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2405,7 +2412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2440,7 +2447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -6395,7 +6402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -6429,8 +6436,9 @@
       <c r="K145" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L145" s="1"/>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -6465,7 +6473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -6500,7 +6508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -6535,7 +6543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -6570,7 +6578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -6605,7 +6613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -6640,7 +6648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -6675,7 +6683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -6710,7 +6718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -6745,7 +6753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -6780,7 +6788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -6815,7 +6823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -6850,7 +6858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -6885,7 +6893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -6920,7 +6928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -7515,7 +7523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -7550,7 +7558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -7585,7 +7593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -7620,7 +7628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -7655,7 +7663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -7690,7 +7698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
@@ -7725,7 +7733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
@@ -7760,7 +7768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -7795,7 +7803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
@@ -7830,7 +7838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
@@ -7865,7 +7873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
@@ -7899,8 +7907,9 @@
       <c r="K187" s="1" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L187" s="1"/>
+    </row>
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -7935,7 +7944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
@@ -7970,7 +7979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
@@ -8005,7 +8014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
@@ -8040,7 +8049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
@@ -10037,7 +10046,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>